<commit_message>
updated hierlinreg to work better with dfs, reran hist word order stats
</commit_message>
<xml_diff>
--- a/scripts/checks/results/HLR_results_XX_All_lg_families_random_tPBC.xlsx
+++ b/scripts/checks/results/HLR_results_XX_All_lg_families_random_tPBC.xlsx
@@ -567,57 +567,57 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3171711162432754</v>
+        <v>0.3257249711502525</v>
       </c>
       <c r="H2" t="n">
-        <v>156.5350686191314</v>
+        <v>162.7960558837417</v>
       </c>
       <c r="I2" t="n">
-        <v>9.246824925743561e-30</v>
+        <v>1.090967547286175e-30</v>
       </c>
       <c r="J2" t="n">
-        <v>38.32704424815032</v>
+        <v>37.84691813850442</v>
       </c>
       <c r="K2" t="n">
         <v>56.12979351032449</v>
       </c>
       <c r="L2" t="n">
-        <v>17.80274926217417</v>
+        <v>18.28287537182007</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1137301016265588</v>
+        <v>0.1123053950697461</v>
       </c>
       <c r="N2" t="n">
         <v>0.1660644778411967</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>{'const': 0.7854345678146204, 'N1ratio-ArgsPreds': -0.22479130013260132}</t>
+          <t>{'const': 0.8041965056596425, 'N1ratio-ArgsPreds': -0.22818582580893026}</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>{'const': 1.1223535915051682e-42, 'N1ratio-ArgsPreds': 9.24682492574382e-30}</t>
+          <t>{'const': 1.5299431630824037e-43, 'N1ratio-ArgsPreds': 1.090967547286159e-30}</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': -0.5631794707225003}</t>
+          <t>{'N1ratio-ArgsPreds': -0.5707232001156536}</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(-0.5631794707225021)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(-0.5707232001156564)}</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(-0.5631794707225023)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(-0.5707232001156562)}</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(31.71711162432778)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(32.57249711502554)}</t>
         </is>
       </c>
       <c r="U2" t="inlineStr"/>
@@ -646,67 +646,67 @@
         <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3865258411832952</v>
+        <v>0.4297222340761711</v>
       </c>
       <c r="H3" t="n">
-        <v>52.61005255878809</v>
+        <v>62.91987639958763</v>
       </c>
       <c r="I3" t="n">
-        <v>2.390832756005256e-34</v>
+        <v>1.343846501666787e-39</v>
       </c>
       <c r="J3" t="n">
-        <v>34.43417785830165</v>
+        <v>32.00957324483368</v>
       </c>
       <c r="K3" t="n">
         <v>56.12979351032449</v>
       </c>
       <c r="L3" t="n">
-        <v>5.423903913005709</v>
+        <v>6.030055066372702</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1030963408931187</v>
+        <v>0.09583704564321462</v>
       </c>
       <c r="N3" t="n">
         <v>0.1660644778411967</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>{'const': 0.637931857336678, 'N1ratio-ArgsPreds': -0.2229349133726168, 'latitude': 0.004573501126558595, 'longitude': -0.00018687011325787848, 'Macro_class': 0.04713327394274785}</t>
+          <t>{'const': 0.6460951361165155, 'N1ratio-ArgsPreds': -0.2314807109302169, 'latitude': 0.005203641687904243, 'longitude': -0.0001992181028474547, 'Macro_class': 0.05827317632261819}</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>{'const': 3.996330084738999e-27, 'N1ratio-ArgsPreds': 2.4225090972382558e-29, 'latitude': 1.4261443373003804e-05, 'longitude': 0.42026588548329114, 'Macro_class': 4.902521014871655e-06}</t>
+          <t>{'const': 3.6013124999025194e-29, 'N1ratio-ArgsPreds': 1.047041916647843e-31, 'latitude': 1.7345666833023843e-07, 'longitude': 0.3693533121444341, 'Macro_class': 3.774054689809112e-09}</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': -0.55852858382284, 'latitude': 0.19709963112850895, 'longitude': -0.037881263566533124, 'Macro_class': 0.20463093909330426}</t>
+          <t>{'N1ratio-ArgsPreds': -0.5789641474828611, 'latitude': 0.23003147484609276, 'longitude': -0.04088923999541228, 'Macro_class': 0.2551047618687475}</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(-0.5617821966837733), 'latitude': np.float64(0.23432418278487468), 'longitude': np.float64(-0.04411170654455132), 'Macro_class': np.float64(0.24632179514189084)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(-0.5808785653454406), 'latitude': np.float64(0.28039353684640295), 'longitude': np.float64(-0.049126251090201724), 'Macro_class': np.float64(0.3145097411962766)}</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(-0.5318765783172628), 'latitude': np.float64(0.18878964235675724), 'longitude': np.float64(-0.034583977700257396), 'Macro_class': np.float64(0.19906408167823011)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(-0.5389014838131498), 'latitude': np.float64(0.2205931154493497), 'longitude': np.float64(-0.03714338992437315), 'Macro_class': np.float64(0.25020430209163114)}</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(28.289269456247933), 'latitude': np.float64(3.5641529061192307), 'longitude': np.float64(0.11960515135719008), 'Macro_class': np.float64(3.962650861439707)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(29.04148092560146), 'latitude': np.float64(4.866132258365012), 'longitude': np.float64(0.13796314150740252), 'Macro_class': np.float64(6.260219278516022)}</t>
         </is>
       </c>
       <c r="U3" t="n">
-        <v>0.06935472494001982</v>
+        <v>0.1039972629259186</v>
       </c>
       <c r="V3" t="n">
-        <v>12.58650034238185</v>
+        <v>20.30302184467789</v>
       </c>
       <c r="W3" t="n">
-        <v>8.148462682966074e-08</v>
+        <v>4.134710699016487e-12</v>
       </c>
     </row>
     <row r="4">
@@ -731,67 +731,67 @@
         <v>5</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3866132245385033</v>
+        <v>0.4297976308001815</v>
       </c>
       <c r="H4" t="n">
-        <v>41.97749574058203</v>
+        <v>50.20063710268639</v>
       </c>
       <c r="I4" t="n">
-        <v>1.812199498110855e-33</v>
+        <v>1.114892836579535e-38</v>
       </c>
       <c r="J4" t="n">
-        <v>34.42927304861758</v>
+        <v>32.00534124228362</v>
       </c>
       <c r="K4" t="n">
         <v>56.12979351032449</v>
       </c>
       <c r="L4" t="n">
-        <v>4.340104092341382</v>
+        <v>4.824890453608174</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1033912103562089</v>
+        <v>0.09611213586271357</v>
       </c>
       <c r="N4" t="n">
         <v>0.1660644778411967</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>{'const': 0.6354777292886532, 'N1ratio-ArgsPreds': -0.22407295186328563, 'latitude': 0.004571842200274629, 'longitude': -0.00017196375644886998, 'Macro_class': 0.04686684490455507, 'Fam_class': 0.00011422298199979561}</t>
+          <t>{'const': 0.6478715557735011, 'N1ratio-ArgsPreds': -0.23029823450386092, 'latitude': 0.005210450677401761, 'longitude': -0.0002120248347705356, 'Macro_class': 0.0585405949575478, 'Fam_class': -0.00010656470313954815}</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>{'const': 5.39731004421354e-26, 'N1ratio-ArgsPreds': 1.1264037783223864e-27, 'latitude': 1.4779827436397332e-05, 'longitude': 0.47745636768074806, 'Macro_class': 6.611499743559735e-06, 'Fam_class': 0.8277138940049094}</t>
+          <t>{'const': 1.2519041382639054e-28, 'N1ratio-ArgsPreds': 4.160768616548865e-29, 'latitude': 1.769814041948919e-07, 'longitude': 0.3576527504768595, 'Macro_class': 4.559021367809855e-09, 'Fam_class': 0.8339225463295897}</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': -0.5613797614015925, 'latitude': 0.1970281380317345, 'longitude': -0.03485953033560392, 'Macro_class': 0.20347422707806556, 'Fam_class': 0.009992041305528289}</t>
+          <t>{'N1ratio-ArgsPreds': -0.5760066161475172, 'latitude': 0.2303324721072928, 'longitude': -0.04351780400478214, 'Macro_class': 0.25627545088019416, 'Fam_class': -0.009322107485196199}</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(-0.5482135332660187), 'latitude': np.float64(0.23425368046355935), 'longitude': np.float64(-0.0389441140439864), 'Macro_class': np.float64(0.24337784375364252), 'Fam_class': np.float64(0.011934829555896346)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(-0.5605078062590266), 'latitude': np.float64(0.28060584710727093), 'longitude': np.float64(-0.0504130760596281), 'Macro_class': np.float64(0.3133713427156236), 'Fam_class': np.float64(-0.01149828365769737)}</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(-0.5133752391231147), 'latitude': np.float64(0.18871609993020977), 'longitude': np.float64(-0.03052380128810994), 'Macro_class': np.float64(0.19652018027414628), 'Fam_class': np.float64(0.009347906461237123)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(-0.5110785084455699), 'latitude': np.float64(0.22075982091380303), 'longitude': np.float64(-0.03811626027475098), 'Macro_class': np.float64(0.24918337091065954), 'Fam_class': np.float64(-0.00868312869941237)}</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(26.35541361447152), 'latitude': np.float64(3.5613766372868922), 'longitude': np.float64(0.0931702445076022), 'Macro_class': np.float64(3.8620181254982953), 'Fam_class': np.float64(0.008738335520803876)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(26.120124179494848), 'latitude': np.float64(4.873489852989438), 'longitude': np.float64(0.14528492973325596), 'Macro_class': np.float64(6.209235233839933), 'Fam_class': np.float64(0.007539672401055876)}</t>
         </is>
       </c>
       <c r="U4" t="n">
-        <v>8.73833552080816e-05</v>
+        <v>7.539672401046804e-05</v>
       </c>
       <c r="V4" t="n">
-        <v>0.04743932938951623</v>
+        <v>0.0440319269993904</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8277138940049527</v>
+        <v>0.833922546329686</v>
       </c>
     </row>
     <row r="5">
@@ -816,67 +816,67 @@
         <v>7</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4077971205523294</v>
+        <v>0.4307960039466122</v>
       </c>
       <c r="H5" t="n">
-        <v>32.56143932795307</v>
+        <v>35.78769105502964</v>
       </c>
       <c r="I5" t="n">
-        <v>2.607955351645357e-34</v>
+        <v>4.246057926749762e-37</v>
       </c>
       <c r="J5" t="n">
-        <v>33.24022533961734</v>
+        <v>31.94930276372821</v>
       </c>
       <c r="K5" t="n">
         <v>56.12979351032449</v>
       </c>
       <c r="L5" t="n">
-        <v>3.269938310101022</v>
+        <v>3.454355820942326</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1004236415094179</v>
+        <v>0.09652357330431482</v>
       </c>
       <c r="N5" t="n">
         <v>0.1660644778411967</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>{'const': 0.49284857671486215, 'N1ratio-ArgsPreds': -0.20952419733975422, 'latitude': 0.0047675225866093685, 'longitude': -0.0002526002680744043, 'Macro_class': 0.03420852390113951, 'Fam_class': -0.0005284344427297379, 'Nlen_freq': -0.04094499883153864, 'Vlen_freq': 0.06902203448192538}</t>
+          <t>{'const': 0.623312746996375, 'N1ratio-ArgsPreds': -0.22791442762176128, 'latitude': 0.005240558481256999, 'longitude': -0.00020654660329224965, 'Macro_class': 0.055688107563884884, 'Fam_class': -0.00021841796015278017, 'Nlen_freq': -0.010433171531082964, 'Vlen_freq': 0.01555204247010605}</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>{'const': 8.416326099571912e-06, 'N1ratio-ArgsPreds': 2.6024800763715207e-24, 'latitude': 4.919705086089294e-06, 'longitude': 0.30958950581200456, 'Macro_class': 0.0015801026362803332, 'Fam_class': 0.3407886947043749, 'Nlen_freq': 0.12086044789552168, 'Vlen_freq': 0.0027398857188410666}</t>
+          <t>{'const': 2.9487034745625933e-09, 'N1ratio-ArgsPreds': 1.0481199564811615e-27, 'latitude': 1.699262448169016e-07, 'longitude': 0.3813401191945358, 'Macro_class': 1.8222686347441684e-07, 'Fam_class': 0.6813765951816662, 'Nlen_freq': 0.6739099236055167, 'Vlen_freq': 0.4791952800585929}</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': -0.5249301307112556, 'latitude': 0.20546118109838896, 'longitude': -0.05120571270109192, 'Macro_class': 0.1485176348960795, 'Fam_class': -0.04622658843759492, 'Nlen_freq': -0.12108770066300058, 'Vlen_freq': 0.2500528948648835}</t>
+          <t>{'N1ratio-ArgsPreds': -0.5700443970333957, 'latitude': 0.23166341357878115, 'longitude': -0.042393404572881224, 'Macro_class': 0.2437880053140677, 'Fam_class': -0.019106849090314564, 'Nlen_freq': -0.0317491461277499, 'Vlen_freq': 0.056714222012008236}</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(-0.5185186752914335), 'latitude': np.float64(0.24736394731373282), 'longitude': np.float64(-0.05584758062379788), 'Macro_class': np.float64(0.17249158307458), 'Fam_class': np.float64(-0.052363678656906845), 'Nlen_freq': np.float64(-0.08516944894214515), 'Vlen_freq': np.float64(0.16366001942982744)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(-0.5498644558342528), 'latitude': np.float64(0.281808191839382), 'longitude': np.float64(-0.048126418204418056), 'Macro_class': np.float64(0.2811394426544442), 'Fam_class': np.float64(-0.02258198396726297), 'Nlen_freq': np.float64(-0.023142972856167343), 'Vlen_freq': np.float64(0.038907718982092054)}</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(-0.4666592386003867), 'latitude': np.float64(0.19646380781444367), 'longitude': np.float64(-0.043044528140496856), 'Macro_class': np.float64(0.13476033706820037), 'Fam_class': np.float64(-0.0403516810479265), 'Nlen_freq': np.float64(-0.06578092643699414), 'Vlen_freq': np.float64(0.12766544692590626)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(-0.4966736319771695), 'latitude': np.float64(0.22159289869439136), 'longitude': np.float64(-0.03635139152273897), 'Macro_class': np.float64(0.22102185575082223), 'Fam_class': np.float64(-0.01704146105947908), 'Nlen_freq': np.float64(-0.01746503461640957), 'Vlen_freq': np.float64(0.029376409226563177)}</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>{'N1ratio-ArgsPreds': np.float64(21.777084497109268), 'latitude': np.float64(3.859802778095066), 'longitude': np.float64(0.18528314028380255), 'Macro_class': np.float64(1.816034844673498), 'Fam_class': np.float64(0.1628258163393591), 'Nlen_freq': np.float64(0.43271302829092345), 'Vlen_freq': np.float64(1.6298466338791389)}</t>
+          <t>{'N1ratio-ArgsPreds': np.float64(24.66846967013928), 'latitude': np.float64(4.910341275178279), 'longitude': np.float64(0.13214236656394585), 'Macro_class': np.float64(4.885066071953727), 'Fam_class': np.float64(0.02904113950417418), 'Nlen_freq': np.float64(0.03050274341523846), 'Vlen_freq': np.float64(0.08629734190465062)}</t>
         </is>
       </c>
       <c r="U5" t="n">
-        <v>0.02118389601382609</v>
+        <v>0.0009983731464306977</v>
       </c>
       <c r="V5" t="n">
-        <v>5.920158297031745</v>
+        <v>0.2902838997616293</v>
       </c>
       <c r="W5" t="n">
-        <v>0.002977320531824004</v>
+        <v>0.7482414037482997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>